<commit_message>
Upload Y5_B2526_General_&_Special_Surgery_2_B1_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y5_B2526_General_&_Special_Surgery_2_B1_schedule.xlsx
+++ b/modules_schedules/Y5_B2526_General_&_Special_Surgery_2_B1_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D824D44A-6777-4614-B379-373D2156E27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34AC971-5E9F-4F16-B9CA-A8E3426C4224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="80">
   <si>
     <t>Year</t>
   </si>
@@ -257,6 +257,9 @@
   </si>
   <si>
     <t>B1-9</t>
+  </si>
+  <si>
+    <t>Surgery Seminar/Slide</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="156" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1036,7 +1039,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>41</v>
@@ -1058,8 +1061,8 @@
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
+      <c r="C18" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>44</v>
@@ -1082,7 +1085,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>46</v>
@@ -1104,8 +1107,8 @@
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>9</v>
+      <c r="C20" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>48</v>
@@ -1128,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>50</v>
@@ -1150,8 +1153,8 @@
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>9</v>
+      <c r="C22" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>52</v>
@@ -1174,7 +1177,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>54</v>
@@ -1542,7 +1545,7 @@
         <v>56</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>41</v>
@@ -1564,8 +1567,8 @@
       <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>9</v>
+      <c r="C40" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>44</v>
@@ -1588,7 +1591,7 @@
         <v>56</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>46</v>
@@ -1610,8 +1613,8 @@
       <c r="B42" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>9</v>
+      <c r="C42" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>48</v>
@@ -1634,7 +1637,7 @@
         <v>56</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>50</v>
@@ -1656,8 +1659,8 @@
       <c r="B44" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>9</v>
+      <c r="C44" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>52</v>
@@ -1680,7 +1683,7 @@
         <v>56</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>54</v>
@@ -2048,7 +2051,7 @@
         <v>69</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>41</v>
@@ -2070,8 +2073,8 @@
       <c r="B62" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>9</v>
+      <c r="C62" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>44</v>
@@ -2094,7 +2097,7 @@
         <v>69</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>46</v>
@@ -2116,8 +2119,8 @@
       <c r="B64" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>9</v>
+      <c r="C64" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>48</v>
@@ -2140,7 +2143,7 @@
         <v>69</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>50</v>
@@ -2162,8 +2165,8 @@
       <c r="B66" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>9</v>
+      <c r="C66" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>52</v>
@@ -2186,7 +2189,7 @@
         <v>69</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>54</v>
@@ -2554,7 +2557,7 @@
         <v>70</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>41</v>
@@ -2576,8 +2579,8 @@
       <c r="B84" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>9</v>
+      <c r="C84" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>44</v>
@@ -2600,7 +2603,7 @@
         <v>70</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>46</v>
@@ -2622,8 +2625,8 @@
       <c r="B86" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>9</v>
+      <c r="C86" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>48</v>
@@ -2646,7 +2649,7 @@
         <v>70</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D87" s="6" t="s">
         <v>50</v>
@@ -2668,8 +2671,8 @@
       <c r="B88" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>9</v>
+      <c r="C88" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>52</v>
@@ -2692,7 +2695,7 @@
         <v>70</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D89" s="6" t="s">
         <v>54</v>
@@ -3060,7 +3063,7 @@
         <v>71</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>41</v>
@@ -3082,8 +3085,8 @@
       <c r="B106" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>9</v>
+      <c r="C106" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>44</v>
@@ -3106,7 +3109,7 @@
         <v>71</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>46</v>
@@ -3128,8 +3131,8 @@
       <c r="B108" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C108" s="2" t="s">
-        <v>9</v>
+      <c r="C108" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>48</v>
@@ -3152,7 +3155,7 @@
         <v>71</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D109" s="6" t="s">
         <v>50</v>
@@ -3174,8 +3177,8 @@
       <c r="B110" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C110" s="2" t="s">
-        <v>9</v>
+      <c r="C110" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>52</v>
@@ -3198,7 +3201,7 @@
         <v>71</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>54</v>
@@ -3566,7 +3569,7 @@
         <v>72</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D127" s="6" t="s">
         <v>41</v>
@@ -3588,8 +3591,8 @@
       <c r="B128" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>9</v>
+      <c r="C128" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>44</v>
@@ -3612,7 +3615,7 @@
         <v>72</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D129" s="6" t="s">
         <v>46</v>
@@ -3634,8 +3637,8 @@
       <c r="B130" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C130" s="2" t="s">
-        <v>9</v>
+      <c r="C130" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>48</v>
@@ -3658,7 +3661,7 @@
         <v>72</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D131" s="6" t="s">
         <v>50</v>
@@ -3680,8 +3683,8 @@
       <c r="B132" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>9</v>
+      <c r="C132" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>52</v>
@@ -3704,7 +3707,7 @@
         <v>72</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>54</v>
@@ -4072,7 +4075,7 @@
         <v>73</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D149" s="6" t="s">
         <v>41</v>
@@ -4094,8 +4097,8 @@
       <c r="B150" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C150" s="2" t="s">
-        <v>9</v>
+      <c r="C150" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>44</v>
@@ -4118,7 +4121,7 @@
         <v>73</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D151" s="6" t="s">
         <v>46</v>
@@ -4140,8 +4143,8 @@
       <c r="B152" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C152" s="2" t="s">
-        <v>9</v>
+      <c r="C152" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D152" s="2" t="s">
         <v>48</v>
@@ -4164,7 +4167,7 @@
         <v>73</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D153" s="6" t="s">
         <v>50</v>
@@ -4186,8 +4189,8 @@
       <c r="B154" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C154" s="2" t="s">
-        <v>9</v>
+      <c r="C154" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>52</v>
@@ -4210,7 +4213,7 @@
         <v>73</v>
       </c>
       <c r="C155" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D155" s="6" t="s">
         <v>54</v>
@@ -4578,7 +4581,7 @@
         <v>74</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D171" s="6" t="s">
         <v>41</v>
@@ -4600,8 +4603,8 @@
       <c r="B172" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C172" s="2" t="s">
-        <v>9</v>
+      <c r="C172" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>44</v>
@@ -4624,7 +4627,7 @@
         <v>74</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D173" s="6" t="s">
         <v>46</v>
@@ -4646,8 +4649,8 @@
       <c r="B174" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C174" s="2" t="s">
-        <v>9</v>
+      <c r="C174" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>48</v>
@@ -4670,7 +4673,7 @@
         <v>74</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D175" s="6" t="s">
         <v>50</v>
@@ -4692,8 +4695,8 @@
       <c r="B176" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C176" s="2" t="s">
-        <v>9</v>
+      <c r="C176" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>52</v>
@@ -4716,7 +4719,7 @@
         <v>74</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>54</v>
@@ -5084,7 +5087,7 @@
         <v>75</v>
       </c>
       <c r="C193" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D193" s="6" t="s">
         <v>41</v>
@@ -5106,8 +5109,8 @@
       <c r="B194" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C194" s="2" t="s">
-        <v>9</v>
+      <c r="C194" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>44</v>
@@ -5130,7 +5133,7 @@
         <v>75</v>
       </c>
       <c r="C195" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D195" s="6" t="s">
         <v>46</v>
@@ -5152,8 +5155,8 @@
       <c r="B196" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C196" s="2" t="s">
-        <v>9</v>
+      <c r="C196" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>48</v>
@@ -5176,7 +5179,7 @@
         <v>75</v>
       </c>
       <c r="C197" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D197" s="6" t="s">
         <v>50</v>
@@ -5198,8 +5201,8 @@
       <c r="B198" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C198" s="2" t="s">
-        <v>9</v>
+      <c r="C198" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>52</v>
@@ -5222,7 +5225,7 @@
         <v>75</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D199" s="6" t="s">
         <v>54</v>
@@ -5590,7 +5593,7 @@
         <v>76</v>
       </c>
       <c r="C215" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D215" s="6" t="s">
         <v>41</v>
@@ -5612,8 +5615,8 @@
       <c r="B216" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C216" s="2" t="s">
-        <v>9</v>
+      <c r="C216" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>44</v>
@@ -5636,7 +5639,7 @@
         <v>76</v>
       </c>
       <c r="C217" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D217" s="6" t="s">
         <v>46</v>
@@ -5658,8 +5661,8 @@
       <c r="B218" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C218" s="2" t="s">
-        <v>9</v>
+      <c r="C218" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D218" s="2" t="s">
         <v>48</v>
@@ -5682,7 +5685,7 @@
         <v>76</v>
       </c>
       <c r="C219" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D219" s="6" t="s">
         <v>50</v>
@@ -5704,8 +5707,8 @@
       <c r="B220" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C220" s="2" t="s">
-        <v>9</v>
+      <c r="C220" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D220" s="2" t="s">
         <v>52</v>
@@ -5728,7 +5731,7 @@
         <v>76</v>
       </c>
       <c r="C221" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D221" s="6" t="s">
         <v>54</v>
@@ -6096,7 +6099,7 @@
         <v>77</v>
       </c>
       <c r="C237" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D237" s="6" t="s">
         <v>41</v>
@@ -6118,8 +6121,8 @@
       <c r="B238" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C238" s="2" t="s">
-        <v>9</v>
+      <c r="C238" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D238" s="2" t="s">
         <v>44</v>
@@ -6142,7 +6145,7 @@
         <v>77</v>
       </c>
       <c r="C239" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D239" s="6" t="s">
         <v>46</v>
@@ -6164,8 +6167,8 @@
       <c r="B240" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C240" s="2" t="s">
-        <v>9</v>
+      <c r="C240" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D240" s="2" t="s">
         <v>48</v>
@@ -6188,7 +6191,7 @@
         <v>77</v>
       </c>
       <c r="C241" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D241" s="6" t="s">
         <v>50</v>
@@ -6210,8 +6213,8 @@
       <c r="B242" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C242" s="2" t="s">
-        <v>9</v>
+      <c r="C242" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D242" s="2" t="s">
         <v>52</v>
@@ -6234,7 +6237,7 @@
         <v>77</v>
       </c>
       <c r="C243" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D243" s="6" t="s">
         <v>54</v>
@@ -6602,7 +6605,7 @@
         <v>78</v>
       </c>
       <c r="C259" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D259" s="6" t="s">
         <v>41</v>
@@ -6624,8 +6627,8 @@
       <c r="B260" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C260" s="2" t="s">
-        <v>9</v>
+      <c r="C260" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D260" s="2" t="s">
         <v>44</v>
@@ -6648,7 +6651,7 @@
         <v>78</v>
       </c>
       <c r="C261" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D261" s="6" t="s">
         <v>46</v>
@@ -6670,8 +6673,8 @@
       <c r="B262" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C262" s="2" t="s">
-        <v>9</v>
+      <c r="C262" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D262" s="2" t="s">
         <v>48</v>
@@ -6694,7 +6697,7 @@
         <v>78</v>
       </c>
       <c r="C263" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D263" s="6" t="s">
         <v>50</v>
@@ -6716,8 +6719,8 @@
       <c r="B264" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C264" s="2" t="s">
-        <v>9</v>
+      <c r="C264" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D264" s="2" t="s">
         <v>52</v>
@@ -6740,7 +6743,7 @@
         <v>78</v>
       </c>
       <c r="C265" s="6" t="s">
-        <v>9</v>
+        <v>79</v>
       </c>
       <c r="D265" s="6" t="s">
         <v>54</v>

</xml_diff>